<commit_message>
Adding checkid 5, long running query blocking others
</commit_message>
<xml_diff>
--- a/sp_AskBrent/sp_AskBrent-CheckID-List.xlsx
+++ b/sp_AskBrent/sp_AskBrent-CheckID-List.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="112">
   <si>
     <t>Backups Not Performed Recently</t>
   </si>
@@ -336,6 +336,27 @@
   </si>
   <si>
     <t>http://BrentOzar.com/go/backups</t>
+  </si>
+  <si>
+    <t>Restore Running</t>
+  </si>
+  <si>
+    <t>SQL Server Internal Maintenance</t>
+  </si>
+  <si>
+    <t>Data File Growing</t>
+  </si>
+  <si>
+    <t>http://BrentOzar.com/go/ifi</t>
+  </si>
+  <si>
+    <t>Query Problems</t>
+  </si>
+  <si>
+    <t>Long-Running Query Blocking Others</t>
+  </si>
+  <si>
+    <t>http://BrentOzar.com/go/blocking</t>
   </si>
 </sst>
 </file>
@@ -409,7 +430,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="10">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -420,8 +441,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -439,8 +461,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="10">
+  <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -448,6 +471,7 @@
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Heading 1" xfId="6" builtinId="16"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1389,13 +1413,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomRight" activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1472,12 +1496,66 @@
         <v>103</v>
       </c>
     </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="4">
+        <v>3</v>
+      </c>
+      <c r="B7" s="5">
+        <v>1</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="4">
+        <v>4</v>
+      </c>
+      <c r="B8" s="5">
+        <v>1</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="4">
+        <v>5</v>
+      </c>
+      <c r="B9" s="5">
+        <v>1</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>111</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:E161">
     <sortCondition ref="A2"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="E7" r:id="rId2"/>
+    <hyperlink ref="E8" r:id="rId3"/>
+    <hyperlink ref="E9" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
Adding check ID 6, wait stats
Only uses sys.dm_os_wait_stats, not waiting_tasks yet.
</commit_message>
<xml_diff>
--- a/sp_AskBrent/sp_AskBrent-CheckID-List.xlsx
+++ b/sp_AskBrent/sp_AskBrent-CheckID-List.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="115">
   <si>
     <t>Backups Not Performed Recently</t>
   </si>
@@ -317,9 +317,6 @@
     <t>For updates, visit:</t>
   </si>
   <si>
-    <t>sp_AskBrent Check ID List - v1 June 23, 2013</t>
-  </si>
-  <si>
     <t>http://www.BrentOzar.com/askbrent/documentation/</t>
   </si>
   <si>
@@ -357,6 +354,18 @@
   </si>
   <si>
     <t>http://BrentOzar.com/go/blocking</t>
+  </si>
+  <si>
+    <t>Wait Stats</t>
+  </si>
+  <si>
+    <t>(One per wait type)</t>
+  </si>
+  <si>
+    <t>http://BrentOzar.com/waits/(waittype)</t>
+  </si>
+  <si>
+    <t>sp_AskBrent Check ID List - v1 July 11, 2013</t>
   </si>
 </sst>
 </file>
@@ -1413,13 +1422,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A10" sqref="A10"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1434,7 +1443,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="20" thickBot="1">
       <c r="A1" s="7" t="s">
-        <v>98</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15" thickTop="1">
@@ -1442,7 +1451,7 @@
         <v>97</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="3" customFormat="1">
@@ -1470,13 +1479,13 @@
         <v>1</v>
       </c>
       <c r="C5" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>101</v>
-      </c>
       <c r="E5" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1487,13 +1496,13 @@
         <v>1</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D6" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>102</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1504,13 +1513,13 @@
         <v>1</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1521,13 +1530,13 @@
         <v>1</v>
       </c>
       <c r="C8" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="E8" s="9" t="s">
         <v>107</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1538,13 +1547,30 @@
         <v>1</v>
       </c>
       <c r="C9" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="E9" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="E9" s="6" t="s">
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="4">
+        <v>6</v>
+      </c>
+      <c r="B10" s="5">
+        <v>200</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>111</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CheckID 8, sleeping queries holding locks,
Also moved magic 8 ball to end for readability.
</commit_message>
<xml_diff>
--- a/sp_AskBrent/sp_AskBrent-CheckID-List.xlsx
+++ b/sp_AskBrent/sp_AskBrent-CheckID-List.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
   <si>
     <t>CheckID</t>
   </si>
@@ -94,6 +94,18 @@
   </si>
   <si>
     <t>http://BrentOzar.com/go/freeproccache</t>
+  </si>
+  <si>
+    <t>Query Rolling Back</t>
+  </si>
+  <si>
+    <t>http://BrentOzar.com/go/rollback</t>
+  </si>
+  <si>
+    <t>Sleeping Query with Open Transactions</t>
+  </si>
+  <si>
+    <t>http://BrentOzar.com/go/sleeping</t>
   </si>
 </sst>
 </file>
@@ -167,7 +179,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -175,6 +187,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -199,7 +212,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="12">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -208,6 +221,7 @@
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="Heading 1" xfId="6" builtinId="16"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -509,13 +523,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A12" sqref="A12"/>
+      <selection pane="bottomRight" activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -677,6 +691,40 @@
         <v>24</v>
       </c>
     </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="3">
+        <v>8</v>
+      </c>
+      <c r="B12" s="4">
+        <v>1</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="3">
+        <v>9</v>
+      </c>
+      <c r="B13" s="4">
+        <v>1</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:E161">
     <sortCondition ref="A2"/>
@@ -687,6 +735,8 @@
     <hyperlink ref="E8" r:id="rId3"/>
     <hyperlink ref="E9" r:id="rId4"/>
     <hyperlink ref="E11" r:id="rId5"/>
+    <hyperlink ref="E12" r:id="rId6"/>
+    <hyperlink ref="E13" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
More work on wait stats and Perfmon
</commit_message>
<xml_diff>
--- a/sp_AskBrent/sp_AskBrent-CheckID-List.xlsx
+++ b/sp_AskBrent/sp_AskBrent-CheckID-List.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="35">
   <si>
     <t>CheckID</t>
   </si>
@@ -115,6 +115,15 @@
   </si>
   <si>
     <t>http://BrentOzar.com/go/ple</t>
+  </si>
+  <si>
+    <t>Slow Log File Writes</t>
+  </si>
+  <si>
+    <t>Slow Data File Reads</t>
+  </si>
+  <si>
+    <t>http://BrentOzar.com/go/slow</t>
   </si>
 </sst>
 </file>
@@ -188,7 +197,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="12">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -196,6 +205,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -221,7 +231,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="12">
+  <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -231,6 +241,7 @@
     <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Heading 1" xfId="6" builtinId="16"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -532,13 +543,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A15" sqref="A15"/>
+      <selection pane="bottomRight" activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -751,6 +762,40 @@
         <v>31</v>
       </c>
     </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="3">
+        <v>11</v>
+      </c>
+      <c r="B15" s="4">
+        <v>50</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="3">
+        <v>12</v>
+      </c>
+      <c r="B16" s="4">
+        <v>50</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:E161">
     <sortCondition ref="A2"/>
@@ -764,6 +809,8 @@
     <hyperlink ref="E12" r:id="rId6"/>
     <hyperlink ref="E13" r:id="rId7"/>
     <hyperlink ref="E14" r:id="rId8"/>
+    <hyperlink ref="E15" r:id="rId9"/>
+    <hyperlink ref="E16" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
Adding Perfmon checks, tuning under load at Stack
</commit_message>
<xml_diff>
--- a/sp_AskBrent/sp_AskBrent-CheckID-List.xlsx
+++ b/sp_AskBrent/sp_AskBrent-CheckID-List.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="30360"/>
+    <workbookView xWindow="31940" yWindow="7080" windowWidth="15680" windowHeight="21020"/>
   </bookViews>
   <sheets>
     <sheet name="sp_AskBrent Checks" sheetId="3" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="42">
   <si>
     <t>CheckID</t>
   </si>
@@ -124,6 +124,27 @@
   </si>
   <si>
     <t>http://BrentOzar.com/go/slow</t>
+  </si>
+  <si>
+    <t>Log File Growing</t>
+  </si>
+  <si>
+    <t>http://BrentOzar.com/go/logsize</t>
+  </si>
+  <si>
+    <t>Log File Shrinking</t>
+  </si>
+  <si>
+    <t>Compilations/Sec High</t>
+  </si>
+  <si>
+    <t>http://BrentOzar.com/go/recompile</t>
+  </si>
+  <si>
+    <t>Re-Compilations/Sec High</t>
+  </si>
+  <si>
+    <t>http://BrentOzar.com/go/compile</t>
   </si>
 </sst>
 </file>
@@ -197,7 +218,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -205,6 +226,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -231,7 +255,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="16">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -242,6 +266,9 @@
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
     <cellStyle name="Heading 1" xfId="6" builtinId="16"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -543,13 +570,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A17" sqref="A17"/>
+      <selection pane="bottomRight" activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -796,6 +823,74 @@
         <v>34</v>
       </c>
     </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="3">
+        <v>13</v>
+      </c>
+      <c r="B17" s="4">
+        <v>1</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="3">
+        <v>14</v>
+      </c>
+      <c r="B18" s="4">
+        <v>1</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="3">
+        <v>15</v>
+      </c>
+      <c r="B19" s="4">
+        <v>50</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="3">
+        <v>16</v>
+      </c>
+      <c r="B20" s="4">
+        <v>50</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:E161">
     <sortCondition ref="A2"/>
@@ -811,6 +906,10 @@
     <hyperlink ref="E14" r:id="rId8"/>
     <hyperlink ref="E15" r:id="rId9"/>
     <hyperlink ref="E16" r:id="rId10"/>
+    <hyperlink ref="E17" r:id="rId11"/>
+    <hyperlink ref="E18" r:id="rId12"/>
+    <hyperlink ref="E19" r:id="rId13"/>
+    <hyperlink ref="E20" r:id="rId14"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
v4 work in progress
Added plan cache analysis of queries that ran during the sample. Need
to handle encrypted code & plans, test export as XML, and bail out of
plan analysis if we're more than 5 seconds past the sample duration.
</commit_message>
<xml_diff>
--- a/sp_AskBrent/sp_AskBrent-CheckID-List.xlsx
+++ b/sp_AskBrent/sp_AskBrent-CheckID-List.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="31940" yWindow="7080" windowWidth="15680" windowHeight="21020"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="30360"/>
   </bookViews>
   <sheets>
     <sheet name="sp_AskBrent Checks" sheetId="3" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="45">
   <si>
     <t>CheckID</t>
   </si>
@@ -145,6 +145,15 @@
   </si>
   <si>
     <t>http://BrentOzar.com/go/compile</t>
+  </si>
+  <si>
+    <t>Query Stats</t>
+  </si>
+  <si>
+    <t>Top Resource-Intensive Queries</t>
+  </si>
+  <si>
+    <t>http://BrentOzar.com/go/topqueries</t>
   </si>
 </sst>
 </file>
@@ -570,13 +579,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A21" sqref="A21"/>
+      <selection pane="bottomRight" activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -889,6 +898,23 @@
       </c>
       <c r="E20" s="5" t="s">
         <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="3">
+        <v>17</v>
+      </c>
+      <c r="B21" s="4">
+        <v>210</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -910,6 +936,7 @@
     <hyperlink ref="E18" r:id="rId12"/>
     <hyperlink ref="E19" r:id="rId13"/>
     <hyperlink ref="E20" r:id="rId14"/>
+    <hyperlink ref="E21" r:id="rId15"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
Performance tuning check 8, updating URLs in spreadsheet.
</commit_message>
<xml_diff>
--- a/sp_AskBrent/sp_AskBrent-CheckID-List.xlsx
+++ b/sp_AskBrent/sp_AskBrent-CheckID-List.xlsx
@@ -60,9 +60,6 @@
     <t>Data File Growing</t>
   </si>
   <si>
-    <t>http://BrentOzar.com/go/ifi</t>
-  </si>
-  <si>
     <t>Query Problems</t>
   </si>
   <si>
@@ -157,6 +154,9 @@
   </si>
   <si>
     <t>http://BrentOzar.com/askbrent/dbcc</t>
+  </si>
+  <si>
+    <t>http://BrentOzar.com/go/instant</t>
   </si>
 </sst>
 </file>
@@ -230,7 +230,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="18">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -238,6 +238,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -269,7 +270,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="18">
+  <cellStyles count="19">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -285,6 +286,7 @@
     <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Heading 1" xfId="6" builtinId="16"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -592,7 +594,7 @@
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E7" sqref="E7"/>
+      <selection pane="bottomRight" activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -607,7 +609,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="20" thickBot="1">
       <c r="A1" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15" thickTop="1">
@@ -649,7 +651,7 @@
         <v>8</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -666,7 +668,7 @@
         <v>9</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -683,7 +685,7 @@
         <v>10</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -700,7 +702,7 @@
         <v>12</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>13</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -711,13 +713,13 @@
         <v>1</v>
       </c>
       <c r="C9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="E9" s="5" t="s">
         <v>15</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -728,13 +730,13 @@
         <v>200</v>
       </c>
       <c r="C10" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="E10" s="4" t="s">
         <v>18</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -745,13 +747,13 @@
         <v>50</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D11" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="5" t="s">
         <v>21</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -762,13 +764,13 @@
         <v>1</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D12" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="5" t="s">
         <v>25</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -779,13 +781,13 @@
         <v>1</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D13" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="5" t="s">
         <v>23</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -796,13 +798,13 @@
         <v>50</v>
       </c>
       <c r="C14" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="E14" s="5" t="s">
         <v>28</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -813,13 +815,13 @@
         <v>50</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D15" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" s="5" t="s">
         <v>31</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -830,13 +832,13 @@
         <v>50</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -850,10 +852,10 @@
         <v>11</v>
       </c>
       <c r="D17" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E17" s="5" t="s">
         <v>33</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -867,10 +869,10 @@
         <v>11</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -881,13 +883,13 @@
         <v>50</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -898,13 +900,13 @@
         <v>50</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -915,13 +917,13 @@
         <v>210</v>
       </c>
       <c r="C21" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="E21" s="5" t="s">
         <v>41</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -932,13 +934,13 @@
         <v>210</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
v12 - adding batch requests, wait time
Two new checks in standard output.
</commit_message>
<xml_diff>
--- a/sp_AskBrent/sp_AskBrent-CheckID-List.xlsx
+++ b/sp_AskBrent/sp_AskBrent-CheckID-List.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
+    <workbookView xWindow="18880" yWindow="0" windowWidth="30180" windowHeight="26700"/>
   </bookViews>
   <sheets>
     <sheet name="sp_AskBrent Checks" sheetId="3" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="51">
   <si>
     <t>CheckID</t>
   </si>
@@ -75,12 +75,6 @@
     <t>(One per wait type)</t>
   </si>
   <si>
-    <t>http://BrentOzar.com/waits/(waittype)</t>
-  </si>
-  <si>
-    <t>sp_AskBrent Check ID List - v1 July 11, 2013</t>
-  </si>
-  <si>
     <t>Plan Cache Erased Recently</t>
   </si>
   <si>
@@ -157,6 +151,27 @@
   </si>
   <si>
     <t>http://BrentOzar.com/go/instant</t>
+  </si>
+  <si>
+    <t>sp_AskBrent Check ID List - v12 2015-02-16</t>
+  </si>
+  <si>
+    <t>Server Info</t>
+  </si>
+  <si>
+    <t>Batch Requests per Second</t>
+  </si>
+  <si>
+    <t>http://BrentOzar.com/sql/wait-stats/#(waittype)</t>
+  </si>
+  <si>
+    <t>http://BrentOzar.com/sql/wait-stats/</t>
+  </si>
+  <si>
+    <t>http://BrentOzar.com/go/measure</t>
+  </si>
+  <si>
+    <t>Wait Time per Core per Second</t>
   </si>
 </sst>
 </file>
@@ -230,7 +245,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="19">
+  <cellStyleXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -238,6 +253,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -270,7 +290,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="19">
+  <cellStyles count="24">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -287,6 +307,11 @@
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
     <cellStyle name="Heading 1" xfId="6" builtinId="16"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -588,13 +613,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E11" sqref="E11"/>
+      <selection pane="bottomRight" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -609,7 +634,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="20" thickBot="1">
       <c r="A1" s="6" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15" thickTop="1">
@@ -651,7 +676,7 @@
         <v>8</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -668,7 +693,7 @@
         <v>9</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -685,7 +710,7 @@
         <v>10</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -702,7 +727,7 @@
         <v>12</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -736,7 +761,7 @@
         <v>17</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -750,10 +775,10 @@
         <v>13</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -767,10 +792,10 @@
         <v>13</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -784,10 +809,10 @@
         <v>13</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -798,13 +823,13 @@
         <v>50</v>
       </c>
       <c r="C14" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="5" t="s">
         <v>26</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -815,13 +840,13 @@
         <v>50</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -832,13 +857,13 @@
         <v>50</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D16" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E16" s="5" t="s">
         <v>29</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -852,10 +877,10 @@
         <v>11</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -869,10 +894,10 @@
         <v>11</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -886,10 +911,10 @@
         <v>13</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -903,10 +928,10 @@
         <v>13</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -917,13 +942,13 @@
         <v>210</v>
       </c>
       <c r="C21" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E21" s="5" t="s">
         <v>39</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -934,13 +959,47 @@
         <v>210</v>
       </c>
       <c r="C22" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E22" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D22" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>41</v>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="3">
+        <v>19</v>
+      </c>
+      <c r="B23" s="4">
+        <v>250</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="3">
+        <v>20</v>
+      </c>
+      <c r="B24" s="4">
+        <v>250</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -966,6 +1025,8 @@
     <hyperlink ref="E5" r:id="rId16"/>
     <hyperlink ref="E6" r:id="rId17"/>
     <hyperlink ref="E7" r:id="rId18"/>
+    <hyperlink ref="E24" r:id="rId19"/>
+    <hyperlink ref="E23" r:id="rId20"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
v13 - Option to persist work tables
Add server info output for total data size, number of databases. Added
params to dump file, perfmon, and wait stats work tables to disk.
</commit_message>
<xml_diff>
--- a/sp_AskBrent/sp_AskBrent-CheckID-List.xlsx
+++ b/sp_AskBrent/sp_AskBrent-CheckID-List.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="18880" yWindow="0" windowWidth="30180" windowHeight="26700"/>
+    <workbookView xWindow="53900" yWindow="1840" windowWidth="30180" windowHeight="26700"/>
   </bookViews>
   <sheets>
     <sheet name="sp_AskBrent Checks" sheetId="3" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="53">
   <si>
     <t>CheckID</t>
   </si>
@@ -153,9 +153,6 @@
     <t>http://BrentOzar.com/go/instant</t>
   </si>
   <si>
-    <t>sp_AskBrent Check ID List - v12 2015-02-16</t>
-  </si>
-  <si>
     <t>Server Info</t>
   </si>
   <si>
@@ -172,6 +169,15 @@
   </si>
   <si>
     <t>Wait Time per Core per Second</t>
+  </si>
+  <si>
+    <t>Database Size, Total GB</t>
+  </si>
+  <si>
+    <t>Database Count</t>
+  </si>
+  <si>
+    <t>sp_AskBrent Check ID List - v13 2015-02-22</t>
   </si>
 </sst>
 </file>
@@ -613,13 +619,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C7" sqref="C7"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -634,7 +640,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="20" thickBot="1">
       <c r="A1" s="6" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15" thickTop="1">
@@ -761,7 +767,7 @@
         <v>17</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -976,13 +982,13 @@
         <v>250</v>
       </c>
       <c r="C23" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D23" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D23" s="4" t="s">
-        <v>46</v>
-      </c>
       <c r="E23" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -993,13 +999,41 @@
         <v>250</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D24" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="3">
+        <v>21</v>
+      </c>
+      <c r="B25" s="4">
+        <v>251</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D25" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E24" s="5" t="s">
-        <v>48</v>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="3">
+        <v>22</v>
+      </c>
+      <c r="B26" s="4">
+        <v>251</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixing wait time per core per sec measurements
Because it wasn’t dividing by the number of seconds that had passed.
(sigh)
</commit_message>
<xml_diff>
--- a/sp_AskBrent/sp_AskBrent-CheckID-List.xlsx
+++ b/sp_AskBrent/sp_AskBrent-CheckID-List.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="53900" yWindow="1840" windowWidth="30180" windowHeight="26700"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="sp_AskBrent Checks" sheetId="3" r:id="rId1"/>
@@ -177,7 +177,7 @@
     <t>Database Count</t>
   </si>
   <si>
-    <t>sp_AskBrent Check ID List - v13 2015-02-22</t>
+    <t>sp_AskBrent Check ID List - v14 2015-03-01</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
v14 adding CPU utilization, sorting waits
</commit_message>
<xml_diff>
--- a/sp_AskBrent/sp_AskBrent-CheckID-List.xlsx
+++ b/sp_AskBrent/sp_AskBrent-CheckID-List.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="55">
   <si>
     <t>CheckID</t>
   </si>
@@ -162,9 +162,6 @@
     <t>http://BrentOzar.com/sql/wait-stats/#(waittype)</t>
   </si>
   <si>
-    <t>http://BrentOzar.com/sql/wait-stats/</t>
-  </si>
-  <si>
     <t>http://BrentOzar.com/go/measure</t>
   </si>
   <si>
@@ -178,6 +175,15 @@
   </si>
   <si>
     <t>sp_AskBrent Check ID List - v14 2015-03-01</t>
+  </si>
+  <si>
+    <t>CPU Utilization</t>
+  </si>
+  <si>
+    <t>High CPU Utilization</t>
+  </si>
+  <si>
+    <t>http://BrentOzar.com/go/cpu</t>
   </si>
 </sst>
 </file>
@@ -251,7 +257,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="24">
+  <cellStyleXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -259,6 +265,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -296,7 +306,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="24">
+  <cellStyles count="28">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -318,6 +328,10 @@
     <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
     <cellStyle name="Heading 1" xfId="6" builtinId="16"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -619,13 +633,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -640,7 +654,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="20" thickBot="1">
       <c r="A1" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15" thickTop="1">
@@ -988,7 +1002,7 @@
         <v>45</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -1002,7 +1016,7 @@
         <v>44</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>47</v>
@@ -1019,7 +1033,7 @@
         <v>44</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -1033,7 +1047,38 @@
         <v>44</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="3">
+        <v>23</v>
+      </c>
+      <c r="B27" s="4">
+        <v>251</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="3">
+        <v>24</v>
+      </c>
+      <c r="B28" s="4">
+        <v>50</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1059,8 +1104,9 @@
     <hyperlink ref="E5" r:id="rId16"/>
     <hyperlink ref="E6" r:id="rId17"/>
     <hyperlink ref="E7" r:id="rId18"/>
-    <hyperlink ref="E24" r:id="rId19"/>
-    <hyperlink ref="E23" r:id="rId20"/>
+    <hyperlink ref="E23" r:id="rId19"/>
+    <hyperlink ref="E28" r:id="rId20"/>
+    <hyperlink ref="E24" r:id="rId21"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>